<commit_message>
Update result in real-world projects - final sheet
</commit_message>
<xml_diff>
--- a/Testing_report.xlsx
+++ b/Testing_report.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14640" xr2:uid="{CCB35186-1F36-DB44-9E9C-5585DAC7A179}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" activeTab="1" xr2:uid="{CCB35186-1F36-DB44-9E9C-5585DAC7A179}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="midterm" sheetId="1" r:id="rId1"/>
+    <sheet name="final" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t xml:space="preserve">zt-exec,305172eaed27aa71a6f4de970d20c73cefe6291e,https://github.com/zeroturnaround/zt-exec </t>
   </si>
@@ -111,6 +112,99 @@
   </si>
   <si>
     <t>killed/numberOfMutation</t>
+  </si>
+  <si>
+    <t>Running Time</t>
+  </si>
+  <si>
+    <t>18:16 min</t>
+  </si>
+  <si>
+    <t>404/689</t>
+  </si>
+  <si>
+    <t>0:46 min</t>
+  </si>
+  <si>
+    <t>322/341</t>
+  </si>
+  <si>
+    <t>481/686</t>
+  </si>
+  <si>
+    <t>number of Threads</t>
+  </si>
+  <si>
+    <t>02:54 min</t>
+  </si>
+  <si>
+    <t>02:08 min</t>
+  </si>
+  <si>
+    <t>187/256</t>
+  </si>
+  <si>
+    <t>286/576</t>
+  </si>
+  <si>
+    <t>1290/1655</t>
+  </si>
+  <si>
+    <t>806/1513</t>
+  </si>
+  <si>
+    <t>0:38 min</t>
+  </si>
+  <si>
+    <t>262/292</t>
+  </si>
+  <si>
+    <t>756/945</t>
+  </si>
+  <si>
+    <t>commons-codec</t>
+  </si>
+  <si>
+    <t>commons-lang</t>
+  </si>
+  <si>
+    <t>jfreechart</t>
+  </si>
+  <si>
+    <t>joda-time</t>
+  </si>
+  <si>
+    <t>Project given by TA</t>
+  </si>
+  <si>
+    <t>18:24 min</t>
+  </si>
+  <si>
+    <t>36:16 min</t>
+  </si>
+  <si>
+    <t>1868/2349</t>
+  </si>
+  <si>
+    <t>1243/1874</t>
+  </si>
+  <si>
+    <t>3592/3906</t>
+  </si>
+  <si>
+    <t>14955/19122</t>
+  </si>
+  <si>
+    <t>02:23 h</t>
+  </si>
+  <si>
+    <t>13894/14563</t>
+  </si>
+  <si>
+    <t>35563/48766</t>
+  </si>
+  <si>
+    <t>Got crash when running two last projects, it seems to be too large</t>
   </si>
 </sst>
 </file>
@@ -163,12 +257,30 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -183,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,11 +327,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,14 +671,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B342A164-317F-3B46-9F36-B4F99BC59283}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H9" sqref="B1:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="95" style="3" customWidth="1"/>
+    <col min="2" max="2" width="71" style="3" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" style="1" customWidth="1"/>
@@ -555,28 +689,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10" t="s">
+      <c r="D1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="10"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="16"/>
       <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
@@ -639,7 +773,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -708,7 +842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="38" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -731,7 +865,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="38" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -765,4 +899,342 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C3C96D-FF1B-4442-A4B3-BDA8D9569B5D}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="66.5" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="29.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="19"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.59</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.28898426323319026</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.94</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.73</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="7">
+        <v>28</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.78</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.53</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1">
+        <v>71</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1">
+        <v>51</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0.92</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.78</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="12">
+        <v>106</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.73</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A9:I9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>